<commit_message>
Chapter 5.1 in raport finished.
</commit_message>
<xml_diff>
--- a/Reports/KSR2_Report_Cold_Cloudy.xlsx
+++ b/Reports/KSR2_Report_Cold_Cloudy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
   <si>
     <t>Sentence</t>
   </si>
@@ -158,7 +158,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -200,14 +200,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -224,6 +224,1336 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Report!$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Report!$J$23:$J$37</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Less than quarter</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Some </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Around one thirds </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Around half </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Around two thirds </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Majority </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Almost all</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Less than 200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Around 500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Around 1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Around 2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Around 3000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Around 5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>More than 6000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Report!$K$23:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11604732660214004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96790534679572016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Report!$L$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Report!$J$23:$J$37</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Less than quarter</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Some </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Around one thirds </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Around half </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Around two thirds </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Majority </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Almost all</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Less than 200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Around 500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Around 1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Around 2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Around 3000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Around 5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>More than 6000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Report!$L$23:$L$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95046160774600319</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93244764692636795</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.86489529385273589</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.86489529385273589</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.81986039180364778</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.77482548975455978</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.43704120693537485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Report!$M$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Report!$J$23:$J$37</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Less than quarter</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Some </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Around one thirds </c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Around half </c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Around two thirds </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Majority </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Almost all</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Less than 200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Around 500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Around 1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Around 2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Around 3000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Around 5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>More than 6000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Report!$M$23:$M$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9527133528484576</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.96622382346318392</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.93244764692636795</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93244764692636795</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.90993019590182389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.88741274487727995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.49334609322224721</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="431645088"/>
+        <c:axId val="431645872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="431645088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431645872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="431645872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400">
+                    <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.2764378478664197E-3"/>
+              <c:y val="0.26557079608821138"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431645088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29128014842300559"/>
+          <c:y val="2.6690391459074734E-2"/>
+          <c:w val="0.47464440321583184"/>
+          <c:h val="7.6000831301781216E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="LM Roman 10" panose="00000500000000000000" pitchFamily="50" charset="-18"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5265420</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,31 +1876,31 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.53659085791488403</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.72582972582972582</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.37420846935595864</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
         <v>0.9</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>0.95</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>0.79734294077910384</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="1">
         <v>0.84395406439990994</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>0.95361405088943929</v>
       </c>
       <c r="M3">
@@ -1091,10 +2421,10 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>-1.5895068678225623</v>
+        <v>0.43704120693537485</v>
       </c>
       <c r="I17">
-        <v>-0.5199279441567215</v>
+        <v>0.49334609322224721</v>
       </c>
       <c r="J17">
         <v>0.79734294077910384</v>
@@ -1124,6 +2454,15 @@
         <v>7</v>
       </c>
       <c r="I22" s="1"/>
+      <c r="K22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
@@ -1150,6 +2489,18 @@
       <c r="I23" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
@@ -1176,6 +2527,18 @@
       <c r="I24" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.77500000000000002</v>
+      </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -1202,6 +2565,18 @@
       <c r="I25" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
@@ -1228,6 +2603,18 @@
       <c r="I26" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
@@ -1254,6 +2641,18 @@
       <c r="I27" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
@@ -1280,6 +2679,18 @@
       <c r="I28" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0.11604732660214004</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
@@ -1306,6 +2717,18 @@
       <c r="I29" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.96790534679572016</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
@@ -1332,6 +2755,18 @@
       <c r="I30" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0.87</v>
+      </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
@@ -1358,6 +2793,18 @@
       <c r="I31" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="J31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.95046160774600319</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.9527133528484576</v>
+      </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
@@ -1384,8 +2831,20 @@
       <c r="I32" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0.93244764692636795</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0.96622382346318392</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>39</v>
       </c>
@@ -1410,8 +2869,20 @@
       <c r="I33" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J33" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0.86489529385273589</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.93244764692636795</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
@@ -1436,8 +2907,20 @@
       <c r="I34" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0.86489529385273589</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0.93244764692636795</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>41</v>
       </c>
@@ -1462,8 +2945,20 @@
       <c r="I35" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0.81986039180364778</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0.90993019590182389</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>42</v>
       </c>
@@ -1488,8 +2983,20 @@
       <c r="I36" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0.77482548975455978</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0.88741274487727995</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>43</v>
       </c>
@@ -1503,19 +3010,31 @@
         <v>27</v>
       </c>
       <c r="F37" s="2">
-        <v>-1.5895068678225623</v>
+        <v>0.43704120693537485</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H37" s="2">
-        <v>-0.5199279441567215</v>
+        <v>0.49334609322224721</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.43704120693537485</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0.49334609322224721</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1532,5 +3051,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New diagrams in report.
</commit_message>
<xml_diff>
--- a/Reports/KSR2_Report_Cold_Cloudy.xlsx
+++ b/Reports/KSR2_Report_Cold_Cloudy.xlsx
@@ -66,15 +66,6 @@
     <t>Some of summer measures with cold daily average temperature have cloudy insolation.</t>
   </si>
   <si>
-    <t>Around one thirds of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
-    <t>Around half of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
-    <t>Around two thirds of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
     <t>Majority of summer measures with cold daily average temperature have cloudy insolation.</t>
   </si>
   <si>
@@ -84,21 +75,6 @@
     <t>Less than 200 of summer measures with cold daily average temperature have cloudy insolation.</t>
   </si>
   <si>
-    <t>Around 500 of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
-    <t>Around 1000 of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
-    <t>Around 2000 of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
-    <t>Around 3000 of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
-    <t>Around 5000 of summer measures with cold daily average temperature have cloudy insolation.</t>
-  </si>
-  <si>
     <t>More than 6000 of summer measures with cold daily average temperature have cloudy insolation.</t>
   </si>
   <si>
@@ -120,37 +96,61 @@
     <t xml:space="preserve">Some </t>
   </si>
   <si>
-    <t xml:space="preserve">Around one thirds </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Around half </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Around two thirds </t>
-  </si>
-  <si>
     <t xml:space="preserve">Majority </t>
   </si>
   <si>
     <t>Less than 200</t>
   </si>
   <si>
-    <t>Around 500</t>
-  </si>
-  <si>
-    <t>Around 1000</t>
-  </si>
-  <si>
-    <t>Around 2000</t>
-  </si>
-  <si>
-    <t>Around 3000</t>
-  </si>
-  <si>
-    <t>Around 5000</t>
-  </si>
-  <si>
     <t>More than 6000</t>
+  </si>
+  <si>
+    <t>About one thirds of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t>About half of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t>About two thirds of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t>About 500 of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t>About 1000 of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t>About 2000 of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t>About 3000 of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t>About 5000 of summer measures with cold daily average temperature have cloudy insolation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">About one thirds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">About half </t>
+  </si>
+  <si>
+    <t xml:space="preserve">About two thirds </t>
+  </si>
+  <si>
+    <t>About 500</t>
+  </si>
+  <si>
+    <t>About 1000</t>
+  </si>
+  <si>
+    <t>About 2000</t>
+  </si>
+  <si>
+    <t>About 3000</t>
+  </si>
+  <si>
+    <t>About 5000</t>
   </si>
 </sst>
 </file>
@@ -301,13 +301,13 @@
                   <c:v>Some </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Around one thirds </c:v>
+                  <c:v>About one thirds </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Around half </c:v>
+                  <c:v>About half </c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Around two thirds </c:v>
+                  <c:v>About two thirds </c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Majority </c:v>
@@ -319,19 +319,19 @@
                   <c:v>Less than 200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Around 500</c:v>
+                  <c:v>About 500</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Around 1000</c:v>
+                  <c:v>About 1000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Around 2000</c:v>
+                  <c:v>About 2000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Around 3000</c:v>
+                  <c:v>About 3000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Around 5000</c:v>
+                  <c:v>About 5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>More than 6000</c:v>
@@ -452,13 +452,13 @@
                   <c:v>Some </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Around one thirds </c:v>
+                  <c:v>About one thirds </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Around half </c:v>
+                  <c:v>About half </c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Around two thirds </c:v>
+                  <c:v>About two thirds </c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Majority </c:v>
@@ -470,19 +470,19 @@
                   <c:v>Less than 200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Around 500</c:v>
+                  <c:v>About 500</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Around 1000</c:v>
+                  <c:v>About 1000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Around 2000</c:v>
+                  <c:v>About 2000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Around 3000</c:v>
+                  <c:v>About 3000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Around 5000</c:v>
+                  <c:v>About 5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>More than 6000</c:v>
@@ -600,13 +600,13 @@
                   <c:v>Some </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Around one thirds </c:v>
+                  <c:v>About one thirds </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Around half </c:v>
+                  <c:v>About half </c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Around two thirds </c:v>
+                  <c:v>About two thirds </c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Majority </c:v>
@@ -618,19 +618,19 @@
                   <c:v>Less than 200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Around 500</c:v>
+                  <c:v>About 500</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Around 1000</c:v>
+                  <c:v>About 1000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Around 2000</c:v>
+                  <c:v>About 2000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Around 3000</c:v>
+                  <c:v>About 3000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Around 5000</c:v>
+                  <c:v>About 5000</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>More than 6000</c:v>
@@ -704,11 +704,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="431645088"/>
-        <c:axId val="431645872"/>
+        <c:axId val="430223104"/>
+        <c:axId val="430626432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="431645088"/>
+        <c:axId val="430223104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +751,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="431645872"/>
+        <c:crossAx val="430626432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +759,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="431645872"/>
+        <c:axId val="430626432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,7 +875,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="431645088"/>
+        <c:crossAx val="430223104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1821,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>0.11604732660214004</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>0.96790534679572016</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2365,7 +2365,7 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2466,31 +2466,31 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F23" s="2">
         <v>0.9</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H23" s="2">
         <v>0.95</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K23" s="2">
         <v>0</v>
@@ -2504,31 +2504,31 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D24" s="2">
         <v>0</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F24" s="2">
         <v>0.7</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H24" s="2">
         <v>0.77500000000000002</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="K24" s="2">
         <v>0</v>
@@ -2542,31 +2542,31 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F25" s="2">
         <v>0.75</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H25" s="2">
         <v>0.8</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
@@ -2580,31 +2580,31 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2">
         <v>0.8</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H26" s="2">
         <v>0.9</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K26" s="2">
         <v>0</v>
@@ -2618,31 +2618,31 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F27" s="2">
         <v>0.8</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H27" s="2">
         <v>0.85</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K27" s="2">
         <v>0</v>
@@ -2656,31 +2656,31 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D28" s="2">
         <v>0.11604732660214004</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F28" s="2">
         <v>0.8</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H28" s="2">
         <v>0.9</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K28" s="2">
         <v>0.11604732660214004</v>
@@ -2694,31 +2694,31 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D29" s="2">
         <v>0.96790534679572016</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F29" s="2">
         <v>0.79999999999999993</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H29" s="2">
         <v>0.85</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="K29" s="2">
         <v>0.96790534679572016</v>
@@ -2732,31 +2732,31 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F30" s="2">
         <v>0.84</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H30" s="2">
         <v>0.87</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K30" s="2">
         <v>0</v>
@@ -2770,31 +2770,31 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F31" s="2">
         <v>0.95046160774600319</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H31" s="2">
         <v>0.9527133528484576</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="K31" s="2">
         <v>1</v>
@@ -2808,31 +2808,31 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F32" s="2">
         <v>0.93244764692636795</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H32" s="2">
         <v>0.96622382346318392</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K32" s="2">
         <v>0</v>
@@ -2846,31 +2846,31 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F33" s="2">
         <v>0.86489529385273589</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H33" s="2">
         <v>0.93244764692636795</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K33" s="2">
         <v>0</v>
@@ -2884,31 +2884,31 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D34" s="2">
         <v>0</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F34" s="2">
         <v>0.86489529385273589</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H34" s="2">
         <v>0.93244764692636795</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K34" s="2">
         <v>0</v>
@@ -2922,31 +2922,31 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F35" s="2">
         <v>0.81986039180364778</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H35" s="2">
         <v>0.90993019590182389</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K35" s="2">
         <v>0</v>
@@ -2960,31 +2960,31 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D36" s="2">
         <v>0</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F36" s="2">
         <v>0.77482548975455978</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H36" s="2">
         <v>0.88741274487727995</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K36" s="2">
         <v>0</v>
@@ -2998,31 +2998,31 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F37" s="2">
         <v>0.43704120693537485</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H37" s="2">
         <v>0.49334609322224721</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="K37" s="2">
         <v>0</v>

</xml_diff>